<commit_message>
added making markdown and html summary files
</commit_message>
<xml_diff>
--- a/companies/companies.xlsx
+++ b/companies/companies.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-11960" yWindow="-20140" windowWidth="29860" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="oneline" localSheetId="0">Sheet2!$A$2:$J$75</definedName>
+    <definedName name="oneline" localSheetId="0">Sheet2!$A$2:$K$75</definedName>
   </definedNames>
   <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="413">
   <si>
     <t>590408</t>
   </si>
@@ -1280,6 +1280,18 @@
   </si>
   <si>
     <t>MOREHERE-LINKS</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>http://www.optirtc.com/</t>
   </si>
 </sst>
 </file>
@@ -1314,12 +1326,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1335,7 +1353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1379,6 +1397,22 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1661,138 +1695,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.1640625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.83203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="64" style="5" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="46.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C2" s="9">
         <v>42431</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C3" s="9">
         <v>42454</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="J3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="128" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C4" s="9">
         <v>42628</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1802,378 +1846,414 @@
       <c r="H4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C5" s="9">
         <v>42649</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C6" s="9">
         <v>42650</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C7" s="9">
         <v>42654</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C8" s="9">
         <v>42656</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="J8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C9" s="9">
         <v>42670</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C10" s="9">
         <v>42676</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C11" s="9">
         <v>42677</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C12" s="9">
         <v>42677</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C13" s="9">
         <v>42691</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C14" s="9">
         <v>42709</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C15" s="9">
         <v>42716</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C16" s="9">
         <v>42716</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="E16" s="6" t="s">
         <v>5</v>
       </c>
@@ -2186,157 +2266,172 @@
       <c r="H16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C17" s="9">
         <v>42717</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C18" s="9">
         <v>42718</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="J18" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C19" s="9">
         <v>42719</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="J19" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="K19" s="4" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C20" s="9">
         <v>42745</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="I20" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="J20" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C21" s="9">
         <v>42745</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F21" s="6" t="s">
         <v>5</v>
       </c>
@@ -2346,93 +2441,102 @@
       <c r="H21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C22" s="9">
         <v>42752</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="J22" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="K22" s="4" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C23" s="9">
         <v>42752</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="K23" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C24" s="9">
         <v>42753</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F24" s="6" t="s">
         <v>5</v>
       </c>
@@ -2442,125 +2546,137 @@
       <c r="H24" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C25" s="9">
         <v>42762</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="I25" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="J25" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C26" s="9">
         <v>42766</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="J26" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="160" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C27" s="9">
         <v>42767</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="J27" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C28" s="9">
         <v>42768</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F28" s="6" t="s">
         <v>5</v>
       </c>
@@ -2568,63 +2684,69 @@
         <v>5</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="J28" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="K28" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C29" s="9">
         <v>42772</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="G29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="I29" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="J29" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C30" s="9">
         <v>42774</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F30" s="6" t="s">
         <v>5</v>
       </c>
@@ -2634,93 +2756,102 @@
       <c r="H30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="I30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="K30" s="4" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C31" s="9">
         <v>42802</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="J31" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C32" s="9">
         <v>42803</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="I32" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="J32" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C33" s="9">
         <v>42804</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="D33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F33" s="6" t="s">
         <v>5</v>
       </c>
@@ -2730,637 +2861,697 @@
       <c r="H33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="I33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="K33" s="4" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C34" s="9">
         <v>42808</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H34" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="K34" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C35" s="9">
         <v>42816</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="I35" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="J35" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="K35" s="4" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C36" s="9">
         <v>42817</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F36" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="I36" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="J36" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C37" s="9">
         <v>42831</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="J37" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="K37" s="4" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C38" s="9">
         <v>42832</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="I38" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="J38" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="K38" s="4" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C39" s="9">
         <v>42836</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="G39" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="H39" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="I39" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="J39" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C40" s="9">
         <v>42843</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="I40" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I40" s="13" t="s">
+      <c r="J40" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="K40" s="4" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="112" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C41" s="9">
         <v>42846</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="G41" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="J41" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="K41" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C42" s="9">
         <v>42851</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="J42" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C43" s="9">
         <v>42857</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="F43" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="I43" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="I43" s="13" t="s">
+      <c r="J43" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C44" s="9">
         <v>42858</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="J44" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="K44" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C45" s="9">
         <v>42865</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="F45" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="G45" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="G45" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="I45" s="13" t="s">
+      <c r="J45" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C46" s="9">
         <v>42880</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="F46" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="G46" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="H46" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="I46" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="J46" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="K46" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C47" s="9">
         <v>42892</v>
       </c>
-      <c r="C47" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="H47" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H47" s="6" t="s">
+      <c r="I47" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="J47" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="K47" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C48" s="9">
         <v>42894</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="H48" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="I48" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="I48" s="13" t="s">
+      <c r="J48" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="K48" s="4" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C49" s="9">
         <v>42894</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H49" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I49" s="13" t="s">
+      <c r="I49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="K49" s="4" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C50" s="9">
         <v>42394</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="H50" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H50" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I50" s="13" t="s">
+      <c r="I50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="K50" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C51" s="9">
         <v>42395</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="G51" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H51" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I51" s="13" t="s">
+      <c r="I51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="J51" s="4" t="s">
+      <c r="K51" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C52" s="9">
         <v>42411</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="E52" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="E52" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F52" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H52" s="6" t="s">
+      <c r="I52" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="I52" s="13" t="s">
+      <c r="J52" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="K52" s="4" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C53" s="9">
         <v>42422</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="E53" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F53" s="6" t="s">
         <v>5</v>
       </c>
@@ -3370,381 +3561,417 @@
       <c r="H53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="13" t="s">
+      <c r="I53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J53" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C54" s="9">
         <v>42467</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="F54" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="G54" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="H54" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="I54" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="I54" s="13" t="s">
+      <c r="J54" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="K54" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C55" s="9">
         <v>42517</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="D55" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="E55" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="F55" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F55" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="G55" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I55" s="13" t="s">
+      <c r="I55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J55" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="K55" s="4" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C56" s="9">
         <v>42523</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="F56" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="G56" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="H56" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="I56" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I56" s="13" t="s">
+      <c r="J56" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="J56" s="4" t="s">
+      <c r="K56" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C57" s="9">
         <v>42531</v>
       </c>
-      <c r="C57" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="F57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="H57" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="I57" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="I57" s="13" t="s">
+      <c r="J57" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="J57" s="4" t="s">
+      <c r="K57" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B58" s="9">
+      <c r="B58" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C58" s="9">
         <v>42536</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="F58" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F58" s="6" t="s">
+      <c r="G58" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="G58" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I58" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="I58" s="13" t="s">
+      <c r="J58" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="K58" s="4" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C59" s="9">
         <v>42543</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="F59" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F59" s="6" t="s">
+      <c r="G59" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="H59" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H59" s="6" t="s">
+      <c r="I59" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="I59" s="13" t="s">
+      <c r="J59" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="K59" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B60" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C60" s="9">
         <v>42615</v>
       </c>
-      <c r="C60" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="F60" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="G60" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="H60" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H60" s="6" t="s">
+      <c r="I60" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="I60" s="13" t="s">
+      <c r="J60" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="K60" s="4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C61" s="9">
         <v>42626</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="D61" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="E61" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="F61" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="G61" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="G61" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H61" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I61" s="13" t="s">
+      <c r="I61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J61" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="K61" s="4" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C62" s="9">
         <v>42670</v>
       </c>
-      <c r="C62" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="G62" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I62" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="I62" s="13" t="s">
+      <c r="J62" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="K62" s="4" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B63" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C63" s="9">
         <v>42676</v>
       </c>
-      <c r="C63" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="F63" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="G63" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G63" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I63" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="I63" s="13" t="s">
+      <c r="J63" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="K63" s="4" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B64" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C64" s="9">
         <v>42691</v>
       </c>
-      <c r="C64" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="F64" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="G64" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="H64" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H64" s="6" t="s">
+      <c r="I64" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="I64" s="13" t="s">
+      <c r="J64" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="J64" s="4" t="s">
+      <c r="K64" s="4" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="B65" s="9">
+      <c r="B65" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C65" s="9">
         <v>42748</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="D65" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="E65" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="E65" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F65" s="6" t="s">
         <v>5</v>
       </c>
@@ -3754,61 +3981,67 @@
       <c r="H65" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I65" s="13" t="s">
+      <c r="I65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J65" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="J65" s="4" t="s">
+      <c r="K65" s="4" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A66" s="11" t="s">
+    <row r="66" spans="1:11" s="20" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A66" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C66" s="16">
         <v>42768</v>
       </c>
-      <c r="C66" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="F66" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="G66" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H66" s="6" t="s">
+      <c r="H66" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="I66" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="J66" s="4" t="s">
+      <c r="J66" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="K66" s="19" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="128" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C67" s="9">
         <v>42774</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="D67" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="E67" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="E67" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F67" s="6" t="s">
         <v>5</v>
       </c>
@@ -3816,347 +4049,374 @@
         <v>5</v>
       </c>
       <c r="H67" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="I67" s="13" t="s">
+      <c r="J67" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="J67" s="4" t="s">
+      <c r="K67" s="4" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A68" s="11" t="s">
+    <row r="68" spans="1:11" s="20" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C68" s="16">
         <v>42808</v>
       </c>
-      <c r="C68" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="E68" s="6" t="s">
+      <c r="F68" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="G68" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="G68" s="6" t="s">
+      <c r="H68" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H68" s="6" t="s">
+      <c r="I68" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="I68" s="13" t="s">
+      <c r="J68" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="J68" s="4" t="s">
+      <c r="K68" s="19" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
+    <row r="69" spans="1:11" s="20" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A69" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C69" s="16">
         <v>42824</v>
       </c>
-      <c r="C69" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" s="6" t="s">
+      <c r="F69" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="G69" s="6" t="s">
+      <c r="H69" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H69" s="6" t="s">
+      <c r="I69" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="I69" s="13" t="s">
+      <c r="J69" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="J69" s="4" t="s">
+      <c r="K69" s="19" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="B70" s="9">
+      <c r="B70" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C70" s="9">
         <v>42832</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="F70" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="G70" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="H70" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H70" s="6" t="s">
+      <c r="I70" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I70" s="13" t="s">
+      <c r="J70" s="13" t="s">
         <v>328</v>
       </c>
-      <c r="J70" s="4" t="s">
+      <c r="K70" s="4" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="B71" s="9">
+      <c r="B71" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C71" s="9">
         <v>42838</v>
       </c>
-      <c r="C71" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="E71" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F71" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G71" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="H71" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="I71" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="I71" s="13" t="s">
+      <c r="J71" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="J71" s="4" t="s">
+      <c r="K71" s="4" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="B72" s="9">
+      <c r="B72" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C72" s="9">
         <v>42838</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="D72" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="E72" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="F72" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F72" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="G72" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I72" s="13" t="s">
+      <c r="I72" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J72" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="J72" s="4" t="s">
+      <c r="K72" s="4" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="96" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C73" s="9">
         <v>42842</v>
       </c>
-      <c r="C73" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="6" t="s">
+      <c r="D73" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="F73" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="F73" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="G73" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I73" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I73" s="13" t="s">
+      <c r="J73" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="J73" s="4" t="s">
+      <c r="K73" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C74" s="9">
         <v>42849</v>
       </c>
-      <c r="C74" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="E74" s="6" t="s">
+      <c r="F74" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="G74" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G74" s="6" t="s">
+      <c r="H74" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H74" s="6" t="s">
+      <c r="I74" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="I74" s="13" t="s">
+      <c r="J74" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="J74" s="4" t="s">
+      <c r="K74" s="4" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C75" s="9">
         <v>42892</v>
       </c>
-      <c r="C75" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75" s="6" t="s">
+      <c r="D75" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="E75" s="6" t="s">
+      <c r="F75" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F75" s="6" t="s">
+      <c r="G75" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G75" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="H75" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I75" s="13" t="s">
+      <c r="I75" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J75" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="K75" s="4" t="s">
         <v>347</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6" location=".6a4h07oyv"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="I11" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I13" r:id="rId12"/>
-    <hyperlink ref="I14" r:id="rId13"/>
-    <hyperlink ref="I15" r:id="rId14"/>
-    <hyperlink ref="I16" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
-    <hyperlink ref="I18" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I20" r:id="rId19"/>
-    <hyperlink ref="I21" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
-    <hyperlink ref="I23" r:id="rId22"/>
-    <hyperlink ref="I24" r:id="rId23"/>
-    <hyperlink ref="I25" r:id="rId24"/>
-    <hyperlink ref="I26" r:id="rId25"/>
-    <hyperlink ref="I27" r:id="rId26" display="http://www.businesswire.com/news/home/20161116006061/en/Petuum-Revolutionary-AIML-Development-Platform-Closes-15"/>
-    <hyperlink ref="I28" r:id="rId27"/>
-    <hyperlink ref="I29" r:id="rId28"/>
-    <hyperlink ref="I30" r:id="rId29"/>
-    <hyperlink ref="I31" r:id="rId30"/>
-    <hyperlink ref="I32" r:id="rId31"/>
-    <hyperlink ref="I33" r:id="rId32"/>
-    <hyperlink ref="I34" r:id="rId33"/>
-    <hyperlink ref="I35" r:id="rId34"/>
-    <hyperlink ref="I36" r:id="rId35"/>
-    <hyperlink ref="I37" r:id="rId36"/>
-    <hyperlink ref="I38" r:id="rId37"/>
-    <hyperlink ref="I39" r:id="rId38"/>
-    <hyperlink ref="I40" r:id="rId39"/>
-    <hyperlink ref="I41" r:id="rId40"/>
-    <hyperlink ref="I42" r:id="rId41"/>
-    <hyperlink ref="I43" r:id="rId42"/>
-    <hyperlink ref="I44" r:id="rId43"/>
-    <hyperlink ref="I45" r:id="rId44"/>
-    <hyperlink ref="I46" r:id="rId45"/>
-    <hyperlink ref="I47" r:id="rId46"/>
-    <hyperlink ref="I48" r:id="rId47"/>
-    <hyperlink ref="I49" r:id="rId48"/>
-    <hyperlink ref="I50" r:id="rId49"/>
-    <hyperlink ref="I51" r:id="rId50"/>
-    <hyperlink ref="I52" r:id="rId51"/>
-    <hyperlink ref="I53" r:id="rId52"/>
-    <hyperlink ref="I54" r:id="rId53"/>
-    <hyperlink ref="I55" r:id="rId54"/>
-    <hyperlink ref="I56" r:id="rId55"/>
-    <hyperlink ref="I57" r:id="rId56"/>
-    <hyperlink ref="I58" r:id="rId57"/>
-    <hyperlink ref="I59" r:id="rId58"/>
-    <hyperlink ref="I60" r:id="rId59"/>
-    <hyperlink ref="I61" r:id="rId60"/>
-    <hyperlink ref="I62" r:id="rId61"/>
-    <hyperlink ref="I63" r:id="rId62"/>
-    <hyperlink ref="I64" r:id="rId63"/>
-    <hyperlink ref="I65" r:id="rId64"/>
-    <hyperlink ref="I66" r:id="rId65"/>
-    <hyperlink ref="I67" r:id="rId66"/>
-    <hyperlink ref="I68" r:id="rId67"/>
-    <hyperlink ref="I69" r:id="rId68"/>
-    <hyperlink ref="I70" r:id="rId69"/>
-    <hyperlink ref="I71" r:id="rId70"/>
-    <hyperlink ref="I72" r:id="rId71"/>
-    <hyperlink ref="I73" r:id="rId72"/>
-    <hyperlink ref="I74" r:id="rId73"/>
-    <hyperlink ref="I75" r:id="rId74"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6" location=".6a4h07oyv"/>
+    <hyperlink ref="J8" r:id="rId7"/>
+    <hyperlink ref="J9" r:id="rId8"/>
+    <hyperlink ref="J10" r:id="rId9"/>
+    <hyperlink ref="J11" r:id="rId10"/>
+    <hyperlink ref="J12" r:id="rId11"/>
+    <hyperlink ref="J13" r:id="rId12"/>
+    <hyperlink ref="J14" r:id="rId13"/>
+    <hyperlink ref="J15" r:id="rId14"/>
+    <hyperlink ref="J16" r:id="rId15"/>
+    <hyperlink ref="J17" r:id="rId16"/>
+    <hyperlink ref="J18" r:id="rId17"/>
+    <hyperlink ref="J19" r:id="rId18"/>
+    <hyperlink ref="J20" r:id="rId19"/>
+    <hyperlink ref="J21" r:id="rId20"/>
+    <hyperlink ref="J22" r:id="rId21"/>
+    <hyperlink ref="J23" r:id="rId22"/>
+    <hyperlink ref="J24" r:id="rId23"/>
+    <hyperlink ref="J25" r:id="rId24"/>
+    <hyperlink ref="J26" r:id="rId25"/>
+    <hyperlink ref="J27" r:id="rId26" display="http://www.businesswire.com/news/home/20161116006061/en/Petuum-Revolutionary-AIML-Development-Platform-Closes-15"/>
+    <hyperlink ref="J28" r:id="rId27"/>
+    <hyperlink ref="J29" r:id="rId28"/>
+    <hyperlink ref="J30" r:id="rId29"/>
+    <hyperlink ref="J31" r:id="rId30"/>
+    <hyperlink ref="J32" r:id="rId31"/>
+    <hyperlink ref="J33" r:id="rId32"/>
+    <hyperlink ref="J34" r:id="rId33"/>
+    <hyperlink ref="J35" r:id="rId34"/>
+    <hyperlink ref="J36" r:id="rId35"/>
+    <hyperlink ref="J37" r:id="rId36"/>
+    <hyperlink ref="J38" r:id="rId37"/>
+    <hyperlink ref="J39" r:id="rId38"/>
+    <hyperlink ref="J40" r:id="rId39"/>
+    <hyperlink ref="J41" r:id="rId40"/>
+    <hyperlink ref="J42" r:id="rId41"/>
+    <hyperlink ref="J43" r:id="rId42"/>
+    <hyperlink ref="J44" r:id="rId43"/>
+    <hyperlink ref="J45" r:id="rId44"/>
+    <hyperlink ref="J46" r:id="rId45"/>
+    <hyperlink ref="J47" r:id="rId46"/>
+    <hyperlink ref="J48" r:id="rId47"/>
+    <hyperlink ref="J49" r:id="rId48"/>
+    <hyperlink ref="J50" r:id="rId49"/>
+    <hyperlink ref="J51" r:id="rId50"/>
+    <hyperlink ref="J52" r:id="rId51"/>
+    <hyperlink ref="J53" r:id="rId52"/>
+    <hyperlink ref="J54" r:id="rId53"/>
+    <hyperlink ref="J55" r:id="rId54"/>
+    <hyperlink ref="J56" r:id="rId55"/>
+    <hyperlink ref="J57" r:id="rId56"/>
+    <hyperlink ref="J58" r:id="rId57"/>
+    <hyperlink ref="J59" r:id="rId58"/>
+    <hyperlink ref="J60" r:id="rId59"/>
+    <hyperlink ref="J61" r:id="rId60"/>
+    <hyperlink ref="J62" r:id="rId61"/>
+    <hyperlink ref="J63" r:id="rId62"/>
+    <hyperlink ref="J64" r:id="rId63"/>
+    <hyperlink ref="J65" r:id="rId64"/>
+    <hyperlink ref="J67" r:id="rId65"/>
+    <hyperlink ref="J68" r:id="rId66"/>
+    <hyperlink ref="J69" r:id="rId67"/>
+    <hyperlink ref="J70" r:id="rId68"/>
+    <hyperlink ref="J71" r:id="rId69"/>
+    <hyperlink ref="J72" r:id="rId70"/>
+    <hyperlink ref="J73" r:id="rId71"/>
+    <hyperlink ref="J74" r:id="rId72"/>
+    <hyperlink ref="J75" r:id="rId73"/>
+    <hyperlink ref="J66" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>